<commit_message>
Fixed data, fixed error
</commit_message>
<xml_diff>
--- a/src/WebMarket/WebMarket/App_Data/Batterry.xlsx
+++ b/src/WebMarket/WebMarket/App_Data/Batterry.xlsx
@@ -513,9 +513,6 @@
     <t>Photo</t>
   </si>
   <si>
-    <t>IsAvailable</t>
-  </si>
-  <si>
     <t>Discount</t>
   </si>
   <si>
@@ -922,6 +919,9 @@
   </si>
   <si>
     <t>BB</t>
+  </si>
+  <si>
+    <t>Availability</t>
   </si>
 </sst>
 </file>
@@ -965,8 +965,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1616,28 +1619,29 @@
   <dimension ref="A1:S107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D1" t="s">
         <v>75</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>211</v>
       </c>
       <c r="E1" t="s">
         <v>74</v>
@@ -1676,7 +1680,7 @@
         <v>63</v>
       </c>
       <c r="Q1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R1" t="s">
         <v>62</v>
@@ -1692,8 +1696,8 @@
       <c r="B2">
         <v>4.8</v>
       </c>
-      <c r="D2" t="b">
-        <v>1</v>
+      <c r="D2">
+        <v>0</v>
       </c>
       <c r="E2" t="s">
         <v>59</v>
@@ -1727,8 +1731,8 @@
       <c r="B3">
         <v>5.4</v>
       </c>
-      <c r="D3" t="b">
-        <v>1</v>
+      <c r="D3">
+        <v>0</v>
       </c>
       <c r="E3" t="s">
         <v>56</v>
@@ -1762,8 +1766,8 @@
       <c r="B4">
         <v>5.4</v>
       </c>
-      <c r="D4" t="b">
-        <v>1</v>
+      <c r="D4">
+        <v>0</v>
       </c>
       <c r="E4" t="s">
         <v>53</v>
@@ -1797,8 +1801,8 @@
       <c r="B5">
         <v>8.75</v>
       </c>
-      <c r="D5" t="b">
-        <v>1</v>
+      <c r="D5">
+        <v>0</v>
       </c>
       <c r="E5" t="s">
         <v>50</v>
@@ -1832,8 +1836,8 @@
       <c r="B6">
         <v>8.3000000000000007</v>
       </c>
-      <c r="D6" t="b">
-        <v>1</v>
+      <c r="D6">
+        <v>0</v>
       </c>
       <c r="E6" t="s">
         <v>47</v>
@@ -1864,8 +1868,8 @@
       <c r="B7">
         <v>14</v>
       </c>
-      <c r="D7" t="b">
-        <v>1</v>
+      <c r="D7">
+        <v>0</v>
       </c>
       <c r="E7" t="s">
         <v>45</v>
@@ -1896,8 +1900,8 @@
       <c r="B8">
         <v>10.8</v>
       </c>
-      <c r="D8" t="b">
-        <v>1</v>
+      <c r="D8">
+        <v>0</v>
       </c>
       <c r="E8" t="s">
         <v>43</v>
@@ -1931,8 +1935,8 @@
       <c r="B9">
         <v>12.6</v>
       </c>
-      <c r="D9" t="b">
-        <v>1</v>
+      <c r="D9">
+        <v>0</v>
       </c>
       <c r="E9" t="s">
         <v>40</v>
@@ -1969,8 +1973,8 @@
       <c r="B10">
         <v>14.8</v>
       </c>
-      <c r="D10" t="b">
-        <v>1</v>
+      <c r="D10">
+        <v>0</v>
       </c>
       <c r="E10" t="s">
         <v>38</v>
@@ -2007,8 +2011,8 @@
       <c r="B11">
         <v>17.399999999999999</v>
       </c>
-      <c r="D11" t="b">
-        <v>1</v>
+      <c r="D11">
+        <v>0</v>
       </c>
       <c r="E11" t="s">
         <v>36</v>
@@ -2045,8 +2049,8 @@
       <c r="B12">
         <v>25.2</v>
       </c>
-      <c r="D12" t="b">
-        <v>1</v>
+      <c r="D12">
+        <v>0</v>
       </c>
       <c r="E12" t="s">
         <v>33</v>
@@ -2083,8 +2087,8 @@
       <c r="B13">
         <v>40.799999999999997</v>
       </c>
-      <c r="D13" t="b">
-        <v>1</v>
+      <c r="D13">
+        <v>0</v>
       </c>
       <c r="E13" t="s">
         <v>30</v>
@@ -2121,8 +2125,8 @@
       <c r="B14">
         <v>58</v>
       </c>
-      <c r="D14" t="b">
-        <v>1</v>
+      <c r="D14">
+        <v>0</v>
       </c>
       <c r="E14" t="s">
         <v>27</v>
@@ -2159,8 +2163,8 @@
       <c r="B15">
         <v>60</v>
       </c>
-      <c r="D15" t="b">
-        <v>1</v>
+      <c r="D15">
+        <v>0</v>
       </c>
       <c r="E15" t="s">
         <v>25</v>
@@ -2197,8 +2201,8 @@
       <c r="B16">
         <v>156</v>
       </c>
-      <c r="D16" t="b">
-        <v>1</v>
+      <c r="D16">
+        <v>0</v>
       </c>
       <c r="E16" t="s">
         <v>22</v>
@@ -2235,8 +2239,8 @@
       <c r="B17">
         <v>132</v>
       </c>
-      <c r="D17" t="b">
-        <v>1</v>
+      <c r="D17">
+        <v>0</v>
       </c>
       <c r="E17" t="s">
         <v>19</v>
@@ -2273,8 +2277,8 @@
       <c r="B18">
         <v>186</v>
       </c>
-      <c r="D18" t="b">
-        <v>1</v>
+      <c r="D18">
+        <v>0</v>
       </c>
       <c r="E18" t="s">
         <v>16</v>
@@ -2311,8 +2315,8 @@
       <c r="B19">
         <v>252</v>
       </c>
-      <c r="D19" t="b">
-        <v>1</v>
+      <c r="D19">
+        <v>0</v>
       </c>
       <c r="E19" t="s">
         <v>13</v>
@@ -2349,8 +2353,8 @@
       <c r="B20">
         <v>198</v>
       </c>
-      <c r="D20" t="b">
-        <v>1</v>
+      <c r="D20">
+        <v>0</v>
       </c>
       <c r="E20" t="s">
         <v>11</v>
@@ -2387,8 +2391,8 @@
       <c r="B21">
         <v>240</v>
       </c>
-      <c r="D21" t="b">
-        <v>1</v>
+      <c r="D21">
+        <v>0</v>
       </c>
       <c r="E21" t="s">
         <v>8</v>
@@ -2425,8 +2429,8 @@
       <c r="B22">
         <v>270</v>
       </c>
-      <c r="D22" t="b">
-        <v>1</v>
+      <c r="D22">
+        <v>0</v>
       </c>
       <c r="E22" t="s">
         <v>5</v>
@@ -2463,8 +2467,8 @@
       <c r="B23">
         <v>420</v>
       </c>
-      <c r="D23" t="b">
-        <v>1</v>
+      <c r="D23">
+        <v>0</v>
       </c>
       <c r="E23" t="s">
         <v>2</v>
@@ -2496,19 +2500,19 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B24">
         <v>5.86</v>
       </c>
-      <c r="D24" t="b">
-        <v>1</v>
+      <c r="D24">
+        <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I24">
         <v>0</v>
@@ -2520,7 +2524,7 @@
         <v>5</v>
       </c>
       <c r="L24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M24">
         <v>0.31</v>
@@ -2534,19 +2538,19 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B25">
         <v>9.01</v>
       </c>
-      <c r="D25" t="b">
-        <v>1</v>
+      <c r="D25">
+        <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -2558,7 +2562,7 @@
         <v>5</v>
       </c>
       <c r="L25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M25">
         <v>0.66</v>
@@ -2572,19 +2576,19 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B26">
         <v>7.96</v>
       </c>
-      <c r="D26" t="b">
-        <v>1</v>
+      <c r="D26">
+        <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -2596,7 +2600,7 @@
         <v>5</v>
       </c>
       <c r="L26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M26">
         <v>0.75</v>
@@ -2610,19 +2614,19 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B27">
         <v>13.21</v>
       </c>
-      <c r="D27" t="b">
-        <v>1</v>
+      <c r="D27">
+        <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -2634,7 +2638,7 @@
         <v>5</v>
       </c>
       <c r="L27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M27">
         <v>1.17</v>
@@ -2648,19 +2652,19 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B28">
         <v>20.11</v>
       </c>
-      <c r="D28" t="b">
-        <v>1</v>
+      <c r="D28">
+        <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -2672,7 +2676,7 @@
         <v>5</v>
       </c>
       <c r="L28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M28">
         <v>1.85</v>
@@ -2686,19 +2690,19 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B29">
         <v>10.82</v>
       </c>
-      <c r="D29" t="b">
-        <v>1</v>
+      <c r="D29">
+        <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -2710,7 +2714,7 @@
         <v>5</v>
       </c>
       <c r="L29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M29">
         <v>0.61</v>
@@ -2724,19 +2728,19 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B30">
         <v>13.49</v>
       </c>
-      <c r="D30" t="b">
-        <v>1</v>
+      <c r="D30">
+        <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I30">
         <v>0</v>
@@ -2748,7 +2752,7 @@
         <v>5</v>
       </c>
       <c r="L30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M30">
         <v>1</v>
@@ -2762,19 +2766,19 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B31">
         <v>16.04</v>
       </c>
-      <c r="D31" t="b">
-        <v>1</v>
+      <c r="D31">
+        <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I31">
         <v>0</v>
@@ -2786,7 +2790,7 @@
         <v>5</v>
       </c>
       <c r="L31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M31">
         <v>1.3</v>
@@ -2800,19 +2804,19 @@
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B32">
         <v>16.350000000000001</v>
       </c>
-      <c r="D32" t="b">
-        <v>1</v>
+      <c r="D32">
+        <v>0</v>
       </c>
       <c r="E32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I32">
         <v>0</v>
@@ -2824,7 +2828,7 @@
         <v>5</v>
       </c>
       <c r="L32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M32">
         <v>1.4</v>
@@ -2838,19 +2842,19 @@
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B33">
         <v>18.899999999999999</v>
       </c>
-      <c r="D33" t="b">
-        <v>1</v>
+      <c r="D33">
+        <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I33">
         <v>0</v>
@@ -2862,7 +2866,7 @@
         <v>5</v>
       </c>
       <c r="L33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M33">
         <v>1.7</v>
@@ -2876,19 +2880,19 @@
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B34">
         <v>20.25</v>
       </c>
-      <c r="D34" t="b">
-        <v>1</v>
+      <c r="D34">
+        <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I34">
         <v>0</v>
@@ -2900,7 +2904,7 @@
         <v>5</v>
       </c>
       <c r="L34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M34">
         <v>2.2999999999999998</v>
@@ -2914,19 +2918,19 @@
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B35">
         <v>21.32</v>
       </c>
-      <c r="D35" t="b">
-        <v>1</v>
+      <c r="D35">
+        <v>0</v>
       </c>
       <c r="E35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I35">
         <v>0</v>
@@ -2938,7 +2942,7 @@
         <v>5</v>
       </c>
       <c r="L35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M35">
         <v>2.35</v>
@@ -2952,19 +2956,19 @@
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B36">
         <v>39.01</v>
       </c>
-      <c r="D36" t="b">
-        <v>1</v>
+      <c r="D36">
+        <v>0</v>
       </c>
       <c r="E36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I36">
         <v>0</v>
@@ -2976,7 +2980,7 @@
         <v>5</v>
       </c>
       <c r="L36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M36">
         <v>3.7</v>
@@ -2990,19 +2994,19 @@
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B37">
         <v>55.52</v>
       </c>
-      <c r="D37" t="b">
-        <v>1</v>
+      <c r="D37">
+        <v>0</v>
       </c>
       <c r="E37" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F37" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I37">
         <v>0</v>
@@ -3014,7 +3018,7 @@
         <v>5</v>
       </c>
       <c r="L37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M37">
         <v>5.6</v>
@@ -3028,19 +3032,19 @@
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B38">
         <v>78.040000000000006</v>
       </c>
-      <c r="D38" t="b">
-        <v>1</v>
+      <c r="D38">
+        <v>0</v>
       </c>
       <c r="E38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I38">
         <v>0</v>
@@ -3052,7 +3056,7 @@
         <v>5</v>
       </c>
       <c r="L38" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M38">
         <v>8.4</v>
@@ -3066,31 +3070,31 @@
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B39">
         <v>103.52</v>
       </c>
-      <c r="D39" t="b">
-        <v>1</v>
+      <c r="D39">
+        <v>0</v>
       </c>
       <c r="E39" t="s">
+        <v>92</v>
+      </c>
+      <c r="F39" t="s">
+        <v>92</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>12</v>
+      </c>
+      <c r="K39">
+        <v>5</v>
+      </c>
+      <c r="L39" t="s">
         <v>93</v>
-      </c>
-      <c r="F39" t="s">
-        <v>93</v>
-      </c>
-      <c r="I39">
-        <v>0</v>
-      </c>
-      <c r="J39">
-        <v>12</v>
-      </c>
-      <c r="K39">
-        <v>5</v>
-      </c>
-      <c r="L39" t="s">
-        <v>94</v>
       </c>
       <c r="M39">
         <v>10.5</v>
@@ -3104,19 +3108,19 @@
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B40">
         <v>135.04</v>
       </c>
-      <c r="D40" t="b">
-        <v>1</v>
+      <c r="D40">
+        <v>0</v>
       </c>
       <c r="E40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I40">
         <v>0</v>
@@ -3128,7 +3132,7 @@
         <v>5</v>
       </c>
       <c r="L40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M40">
         <v>13.8</v>
@@ -3142,19 +3146,19 @@
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B41">
         <v>147.06</v>
       </c>
-      <c r="D41" t="b">
-        <v>1</v>
+      <c r="D41">
+        <v>0</v>
       </c>
       <c r="E41" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F41" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I41">
         <v>0</v>
@@ -3166,7 +3170,7 @@
         <v>5</v>
       </c>
       <c r="L41" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M41">
         <v>14</v>
@@ -3180,19 +3184,19 @@
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B42">
         <v>180.06</v>
       </c>
-      <c r="D42" t="b">
-        <v>1</v>
+      <c r="D42">
+        <v>0</v>
       </c>
       <c r="E42" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F42" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I42">
         <v>0</v>
@@ -3204,7 +3208,7 @@
         <v>5</v>
       </c>
       <c r="L42" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M42">
         <v>17</v>
@@ -3218,19 +3222,19 @@
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B43">
         <v>210.07</v>
       </c>
-      <c r="D43" t="b">
-        <v>1</v>
+      <c r="D43">
+        <v>0</v>
       </c>
       <c r="E43" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F43" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I43">
         <v>0</v>
@@ -3242,7 +3246,7 @@
         <v>5</v>
       </c>
       <c r="L43" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M43">
         <v>22</v>
@@ -3256,19 +3260,19 @@
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B44">
         <v>223.56</v>
       </c>
-      <c r="D44" t="b">
-        <v>1</v>
+      <c r="D44">
+        <v>0</v>
       </c>
       <c r="E44" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F44" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I44">
         <v>0</v>
@@ -3280,7 +3284,7 @@
         <v>5</v>
       </c>
       <c r="L44" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M44">
         <v>22.8</v>
@@ -3294,19 +3298,19 @@
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B45">
         <v>231.08</v>
       </c>
-      <c r="D45" t="b">
-        <v>1</v>
+      <c r="D45">
+        <v>0</v>
       </c>
       <c r="E45" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F45" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I45">
         <v>0</v>
@@ -3318,7 +3322,7 @@
         <v>5</v>
       </c>
       <c r="L45" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M45">
         <v>23.5</v>
@@ -3332,19 +3336,19 @@
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B46">
         <v>280.58</v>
       </c>
-      <c r="D46" t="b">
-        <v>1</v>
+      <c r="D46">
+        <v>0</v>
       </c>
       <c r="E46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I46">
         <v>0</v>
@@ -3356,7 +3360,7 @@
         <v>5</v>
       </c>
       <c r="L46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M46">
         <v>28</v>
@@ -3370,19 +3374,19 @@
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B47">
         <v>267.38</v>
       </c>
-      <c r="D47" t="b">
-        <v>1</v>
+      <c r="D47">
+        <v>0</v>
       </c>
       <c r="E47" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F47" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I47">
         <v>0</v>
@@ -3394,7 +3398,7 @@
         <v>5</v>
       </c>
       <c r="L47" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M47">
         <v>32</v>
@@ -3408,19 +3412,19 @@
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B48">
         <v>343.62</v>
       </c>
-      <c r="D48" t="b">
-        <v>1</v>
+      <c r="D48">
+        <v>0</v>
       </c>
       <c r="E48" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F48" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I48">
         <v>0</v>
@@ -3446,19 +3450,19 @@
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B49">
         <v>381.12</v>
       </c>
-      <c r="D49" t="b">
-        <v>1</v>
+      <c r="D49">
+        <v>0</v>
       </c>
       <c r="E49" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F49" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I49">
         <v>0</v>
@@ -3470,7 +3474,7 @@
         <v>5</v>
       </c>
       <c r="L49" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M49">
         <v>43</v>
@@ -3484,19 +3488,19 @@
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B50">
         <v>435.14</v>
       </c>
-      <c r="D50" t="b">
-        <v>1</v>
+      <c r="D50">
+        <v>0</v>
       </c>
       <c r="E50" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F50" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I50">
         <v>0</v>
@@ -3508,7 +3512,7 @@
         <v>5</v>
       </c>
       <c r="L50" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M50">
         <v>45.5</v>
@@ -3522,19 +3526,19 @@
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B51">
         <v>528.16</v>
       </c>
-      <c r="D51" t="b">
-        <v>1</v>
+      <c r="D51">
+        <v>0</v>
       </c>
       <c r="E51" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F51" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I51">
         <v>0</v>
@@ -3546,7 +3550,7 @@
         <v>5</v>
       </c>
       <c r="L51" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M51">
         <v>64</v>
@@ -3560,19 +3564,19 @@
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B52">
         <v>664.59</v>
       </c>
-      <c r="D52" t="b">
-        <v>1</v>
+      <c r="D52">
+        <v>0</v>
       </c>
       <c r="E52" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F52" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I52">
         <v>0</v>
@@ -3584,7 +3588,7 @@
         <v>5</v>
       </c>
       <c r="L52" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M52">
         <v>72.5</v>
@@ -3598,19 +3602,19 @@
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B53">
         <v>20.71</v>
       </c>
-      <c r="D53" t="b">
-        <v>1</v>
+      <c r="D53">
+        <v>0</v>
       </c>
       <c r="E53" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F53" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I53">
         <v>0</v>
@@ -3622,7 +3626,7 @@
         <v>5</v>
       </c>
       <c r="L53" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M53">
         <v>1.8</v>
@@ -3636,19 +3640,19 @@
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B54">
         <v>22.05</v>
       </c>
-      <c r="D54" t="b">
-        <v>1</v>
+      <c r="D54">
+        <v>0</v>
       </c>
       <c r="E54" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F54" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I54">
         <v>0</v>
@@ -3660,7 +3664,7 @@
         <v>5</v>
       </c>
       <c r="L54" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M54">
         <v>1.9</v>
@@ -3674,19 +3678,19 @@
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B55">
         <v>27.31</v>
       </c>
-      <c r="D55" t="b">
-        <v>1</v>
+      <c r="D55">
+        <v>0</v>
       </c>
       <c r="E55" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F55" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I55">
         <v>0</v>
@@ -3698,7 +3702,7 @@
         <v>5</v>
       </c>
       <c r="L55" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M55">
         <v>2.7</v>
@@ -3712,19 +3716,19 @@
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B56">
         <v>177.29</v>
       </c>
-      <c r="D56" t="b">
-        <v>1</v>
+      <c r="D56">
+        <v>0</v>
       </c>
       <c r="E56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I56">
         <v>0</v>
@@ -3736,7 +3740,7 @@
         <v>5</v>
       </c>
       <c r="L56" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M56">
         <v>17.3</v>
@@ -3750,19 +3754,19 @@
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B57">
         <v>277.01</v>
       </c>
-      <c r="D57" t="b">
-        <v>1</v>
+      <c r="D57">
+        <v>0</v>
       </c>
       <c r="E57" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F57" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I57">
         <v>0</v>
@@ -3774,7 +3778,7 @@
         <v>5</v>
       </c>
       <c r="L57" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M57">
         <v>29.4</v>
@@ -3788,19 +3792,19 @@
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B58">
         <v>339.33</v>
       </c>
-      <c r="D58" t="b">
-        <v>1</v>
+      <c r="D58">
+        <v>0</v>
       </c>
       <c r="E58" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F58" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I58">
         <v>0</v>
@@ -3812,7 +3816,7 @@
         <v>5</v>
       </c>
       <c r="L58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M58">
         <v>36</v>
@@ -3826,19 +3830,19 @@
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B59">
         <v>427.98</v>
       </c>
-      <c r="D59" t="b">
-        <v>1</v>
+      <c r="D59">
+        <v>0</v>
       </c>
       <c r="E59" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F59" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I59">
         <v>0</v>
@@ -3850,7 +3854,7 @@
         <v>5</v>
       </c>
       <c r="L59" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M59">
         <v>45.5</v>
@@ -3864,19 +3868,19 @@
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B60">
         <v>8.0500000000000007</v>
       </c>
-      <c r="D60" t="b">
-        <v>1</v>
+      <c r="D60">
+        <v>0</v>
       </c>
       <c r="E60" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F60" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I60">
         <v>0</v>
@@ -3888,7 +3892,7 @@
         <v>5</v>
       </c>
       <c r="L60" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M60">
         <v>0.3</v>
@@ -3902,19 +3906,19 @@
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B61">
         <v>11.68</v>
       </c>
-      <c r="D61" t="b">
-        <v>1</v>
+      <c r="D61">
+        <v>0</v>
       </c>
       <c r="E61" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F61" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I61">
         <v>0</v>
@@ -3926,7 +3930,7 @@
         <v>5</v>
       </c>
       <c r="L61" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="M61">
         <v>0.85</v>
@@ -3940,19 +3944,19 @@
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B62">
         <v>23.95</v>
       </c>
-      <c r="D62" t="b">
-        <v>1</v>
+      <c r="D62">
+        <v>0</v>
       </c>
       <c r="E62" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F62" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I62">
         <v>0</v>
@@ -3964,7 +3968,7 @@
         <v>5</v>
       </c>
       <c r="L62" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M62">
         <v>1.98</v>
@@ -3978,19 +3982,19 @@
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B63">
         <v>13.02</v>
       </c>
-      <c r="D63" t="b">
-        <v>1</v>
+      <c r="D63">
+        <v>0</v>
       </c>
       <c r="E63" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F63" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I63">
         <v>0</v>
@@ -4002,7 +4006,7 @@
         <v>5</v>
       </c>
       <c r="L63" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M63">
         <v>1.3</v>
@@ -4016,19 +4020,19 @@
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B64">
         <v>20.69</v>
       </c>
-      <c r="D64" t="b">
-        <v>1</v>
+      <c r="D64">
+        <v>0</v>
       </c>
       <c r="E64" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F64" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I64">
         <v>0</v>
@@ -4040,7 +4044,7 @@
         <v>5</v>
       </c>
       <c r="L64" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M64">
         <v>1.67</v>
@@ -4054,19 +4058,19 @@
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B65">
         <v>21.74</v>
       </c>
-      <c r="D65" t="b">
-        <v>1</v>
+      <c r="D65">
+        <v>0</v>
       </c>
       <c r="E65" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F65" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I65">
         <v>0</v>
@@ -4078,7 +4082,7 @@
         <v>5</v>
       </c>
       <c r="L65" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M65">
         <v>1.8</v>
@@ -4092,19 +4096,19 @@
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B66">
         <v>26.6</v>
       </c>
-      <c r="D66" t="b">
-        <v>1</v>
+      <c r="D66">
+        <v>0</v>
       </c>
       <c r="E66" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F66" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I66">
         <v>0</v>
@@ -4116,7 +4120,7 @@
         <v>5</v>
       </c>
       <c r="L66" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M66">
         <v>2.54</v>
@@ -4130,19 +4134,19 @@
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B67">
         <v>47.04</v>
       </c>
-      <c r="D67" t="b">
-        <v>1</v>
+      <c r="D67">
+        <v>0</v>
       </c>
       <c r="E67" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F67" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I67">
         <v>0</v>
@@ -4154,7 +4158,7 @@
         <v>5</v>
       </c>
       <c r="L67" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M67">
         <v>3.94</v>
@@ -4168,19 +4172,19 @@
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B68">
         <v>64.08</v>
       </c>
-      <c r="D68" t="b">
-        <v>1</v>
+      <c r="D68">
+        <v>0</v>
       </c>
       <c r="E68" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F68" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I68">
         <v>0</v>
@@ -4192,7 +4196,7 @@
         <v>5</v>
       </c>
       <c r="L68" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M68">
         <v>6.15</v>
@@ -4206,19 +4210,19 @@
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B69">
         <v>66.31</v>
       </c>
-      <c r="D69" t="b">
-        <v>1</v>
+      <c r="D69">
+        <v>0</v>
       </c>
       <c r="E69" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F69" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I69">
         <v>0</v>
@@ -4230,7 +4234,7 @@
         <v>5</v>
       </c>
       <c r="L69" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M69">
         <v>6.35</v>
@@ -4244,19 +4248,19 @@
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B70">
         <v>95.72</v>
       </c>
-      <c r="D70" t="b">
-        <v>1</v>
+      <c r="D70">
+        <v>0</v>
       </c>
       <c r="E70" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F70" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I70">
         <v>0</v>
@@ -4268,7 +4272,7 @@
         <v>5</v>
       </c>
       <c r="L70" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M70">
         <v>9.4</v>
@@ -4282,19 +4286,19 @@
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B71">
         <v>119.06</v>
       </c>
-      <c r="D71" t="b">
-        <v>1</v>
+      <c r="D71">
+        <v>0</v>
       </c>
       <c r="E71" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F71" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I71">
         <v>0</v>
@@ -4306,7 +4310,7 @@
         <v>5</v>
       </c>
       <c r="L71" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M71">
         <v>11.25</v>
@@ -4320,19 +4324,19 @@
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B72">
         <v>152.11000000000001</v>
       </c>
-      <c r="D72" t="b">
-        <v>1</v>
+      <c r="D72">
+        <v>0</v>
       </c>
       <c r="E72" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F72" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I72">
         <v>0</v>
@@ -4344,7 +4348,7 @@
         <v>5</v>
       </c>
       <c r="L72" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M72">
         <v>14.3</v>
@@ -4358,19 +4362,19 @@
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B73">
         <v>241.3</v>
       </c>
-      <c r="D73" t="b">
-        <v>1</v>
+      <c r="D73">
+        <v>0</v>
       </c>
       <c r="E73" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F73" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I73">
         <v>0</v>
@@ -4382,7 +4386,7 @@
         <v>5</v>
       </c>
       <c r="L73" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M73">
         <v>24.5</v>
@@ -4396,19 +4400,19 @@
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B74">
         <v>326.89</v>
       </c>
-      <c r="D74" t="b">
-        <v>1</v>
+      <c r="D74">
+        <v>0</v>
       </c>
       <c r="E74" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F74" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I74">
         <v>0</v>
@@ -4420,7 +4424,7 @@
         <v>5</v>
       </c>
       <c r="L74" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M74">
         <v>30.8</v>
@@ -4434,19 +4438,19 @@
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B75">
         <v>329.71</v>
       </c>
-      <c r="D75" t="b">
-        <v>1</v>
+      <c r="D75">
+        <v>0</v>
       </c>
       <c r="E75" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F75" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I75">
         <v>0</v>
@@ -4458,7 +4462,7 @@
         <v>5</v>
       </c>
       <c r="L75" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M75">
         <v>32.700000000000003</v>
@@ -4472,19 +4476,19 @@
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B76">
         <v>401.55</v>
       </c>
-      <c r="D76" t="b">
-        <v>1</v>
+      <c r="D76">
+        <v>0</v>
       </c>
       <c r="E76" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F76" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I76">
         <v>0</v>
@@ -4496,7 +4500,7 @@
         <v>5</v>
       </c>
       <c r="L76" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="M76">
         <v>39.5</v>
@@ -4510,19 +4514,19 @@
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B77">
         <v>542.24</v>
       </c>
-      <c r="D77" t="b">
-        <v>1</v>
+      <c r="D77">
+        <v>0</v>
       </c>
       <c r="E77" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F77" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I77">
         <v>0</v>
@@ -4534,7 +4538,7 @@
         <v>5</v>
       </c>
       <c r="L77" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="M77">
         <v>51.2</v>
@@ -4548,19 +4552,19 @@
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B78">
         <v>666.67</v>
       </c>
-      <c r="D78" t="b">
-        <v>1</v>
+      <c r="D78">
+        <v>0</v>
       </c>
       <c r="E78" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F78" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I78">
         <v>0</v>
@@ -4572,7 +4576,7 @@
         <v>5</v>
       </c>
       <c r="L78" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M78">
         <v>61.5</v>
@@ -4586,19 +4590,19 @@
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B79">
         <v>705.47</v>
       </c>
-      <c r="D79" t="b">
-        <v>1</v>
+      <c r="D79">
+        <v>0</v>
       </c>
       <c r="E79" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F79" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I79">
         <v>0</v>
@@ -4624,19 +4628,19 @@
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B80">
         <v>18.420000000000002</v>
       </c>
-      <c r="D80" t="b">
-        <v>1</v>
+      <c r="D80">
+        <v>0</v>
       </c>
       <c r="E80" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F80" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I80">
         <v>0</v>
@@ -4648,7 +4652,7 @@
         <v>5</v>
       </c>
       <c r="L80" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M80">
         <v>1.53</v>
@@ -4662,19 +4666,19 @@
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B81">
         <v>22.34</v>
       </c>
-      <c r="D81" t="b">
-        <v>1</v>
+      <c r="D81">
+        <v>0</v>
       </c>
       <c r="E81" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F81" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I81">
         <v>0</v>
@@ -4686,7 +4690,7 @@
         <v>5</v>
       </c>
       <c r="L81" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M81">
         <v>2.2000000000000002</v>
@@ -4700,19 +4704,19 @@
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B82">
         <v>23.37</v>
       </c>
-      <c r="D82" t="b">
-        <v>1</v>
+      <c r="D82">
+        <v>0</v>
       </c>
       <c r="E82" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F82" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I82">
         <v>0</v>
@@ -4724,7 +4728,7 @@
         <v>5</v>
       </c>
       <c r="L82" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M82">
         <v>1.88</v>
@@ -4738,19 +4742,19 @@
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B83">
         <v>30.08</v>
       </c>
-      <c r="D83" t="b">
-        <v>1</v>
+      <c r="D83">
+        <v>0</v>
       </c>
       <c r="E83" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F83" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I83">
         <v>0</v>
@@ -4762,7 +4766,7 @@
         <v>5</v>
       </c>
       <c r="L83" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M83">
         <v>2.1</v>
@@ -4776,19 +4780,19 @@
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B84">
         <v>29.67</v>
       </c>
-      <c r="D84" t="b">
-        <v>1</v>
+      <c r="D84">
+        <v>0</v>
       </c>
       <c r="E84" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F84" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I84">
         <v>0</v>
@@ -4800,7 +4804,7 @@
         <v>5</v>
       </c>
       <c r="L84" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M84">
         <v>2.6</v>
@@ -4814,19 +4818,19 @@
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B85">
         <v>54.04</v>
       </c>
-      <c r="D85" t="b">
-        <v>1</v>
+      <c r="D85">
+        <v>0</v>
       </c>
       <c r="E85" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F85" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I85">
         <v>0</v>
@@ -4838,7 +4842,7 @@
         <v>5</v>
       </c>
       <c r="L85" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M85">
         <v>4.2</v>
@@ -4852,19 +4856,19 @@
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B86">
         <v>81.180000000000007</v>
       </c>
-      <c r="D86" t="b">
-        <v>1</v>
+      <c r="D86">
+        <v>0</v>
       </c>
       <c r="E86" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F86" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I86">
         <v>0</v>
@@ -4876,7 +4880,7 @@
         <v>5</v>
       </c>
       <c r="L86" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M86">
         <v>6.5</v>
@@ -4890,19 +4894,19 @@
     </row>
     <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B87">
         <v>119.73</v>
       </c>
-      <c r="D87" t="b">
-        <v>1</v>
+      <c r="D87">
+        <v>0</v>
       </c>
       <c r="E87" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F87" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I87">
         <v>0</v>
@@ -4914,7 +4918,7 @@
         <v>5</v>
       </c>
       <c r="L87" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M87">
         <v>10</v>
@@ -4928,19 +4932,19 @@
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B88">
         <v>151.78</v>
       </c>
-      <c r="D88" t="b">
-        <v>1</v>
+      <c r="D88">
+        <v>0</v>
       </c>
       <c r="E88" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F88" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I88">
         <v>0</v>
@@ -4952,7 +4956,7 @@
         <v>5</v>
       </c>
       <c r="L88" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M88">
         <v>12.1</v>
@@ -4966,19 +4970,19 @@
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B89">
         <v>181.77</v>
       </c>
-      <c r="D89" t="b">
-        <v>1</v>
+      <c r="D89">
+        <v>0</v>
       </c>
       <c r="E89" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F89" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I89">
         <v>0</v>
@@ -4990,7 +4994,7 @@
         <v>5</v>
       </c>
       <c r="L89" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M89">
         <v>15.3</v>
@@ -5004,19 +5008,19 @@
     </row>
     <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B90">
         <v>244.98</v>
       </c>
-      <c r="D90" t="b">
-        <v>1</v>
+      <c r="D90">
+        <v>0</v>
       </c>
       <c r="E90" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F90" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I90">
         <v>0</v>
@@ -5028,7 +5032,7 @@
         <v>5</v>
       </c>
       <c r="L90" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M90">
         <v>24.75</v>
@@ -5042,19 +5046,19 @@
     </row>
     <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B91">
         <v>243.14</v>
       </c>
-      <c r="D91" t="b">
-        <v>1</v>
+      <c r="D91">
+        <v>0</v>
       </c>
       <c r="E91" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F91" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I91">
         <v>0</v>
@@ -5066,7 +5070,7 @@
         <v>5</v>
       </c>
       <c r="L91" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M91">
         <v>17.8</v>
@@ -5080,19 +5084,19 @@
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B92">
         <v>283.44</v>
       </c>
-      <c r="D92" t="b">
-        <v>1</v>
+      <c r="D92">
+        <v>0</v>
       </c>
       <c r="E92" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F92" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I92">
         <v>0</v>
@@ -5104,7 +5108,7 @@
         <v>5</v>
       </c>
       <c r="L92" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M92">
         <v>26</v>
@@ -5118,19 +5122,19 @@
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B93">
         <v>340.64</v>
       </c>
-      <c r="D93" t="b">
-        <v>1</v>
+      <c r="D93">
+        <v>0</v>
       </c>
       <c r="E93" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F93" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I93">
         <v>0</v>
@@ -5142,7 +5146,7 @@
         <v>5</v>
       </c>
       <c r="L93" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M93">
         <v>29.8</v>
@@ -5156,19 +5160,19 @@
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B94">
         <v>381.82</v>
       </c>
-      <c r="D94" t="b">
-        <v>1</v>
+      <c r="D94">
+        <v>0</v>
       </c>
       <c r="E94" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F94" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I94">
         <v>0</v>
@@ -5180,7 +5184,7 @@
         <v>5</v>
       </c>
       <c r="L94" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M94">
         <v>35</v>
@@ -5194,19 +5198,19 @@
     </row>
     <row r="95" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B95">
         <v>55.26</v>
       </c>
-      <c r="D95" t="b">
-        <v>1</v>
+      <c r="D95">
+        <v>0</v>
       </c>
       <c r="E95" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F95" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I95">
         <v>0</v>
@@ -5218,7 +5222,7 @@
         <v>5</v>
       </c>
       <c r="L95" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M95">
         <v>4.3</v>
@@ -5232,19 +5236,19 @@
     </row>
     <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B96">
         <v>77.36</v>
       </c>
-      <c r="D96" t="b">
-        <v>1</v>
+      <c r="D96">
+        <v>0</v>
       </c>
       <c r="E96" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F96" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I96">
         <v>0</v>
@@ -5256,7 +5260,7 @@
         <v>5</v>
       </c>
       <c r="L96" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M96">
         <v>6.45</v>
@@ -5270,19 +5274,19 @@
     </row>
     <row r="97" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B97">
         <v>169.46</v>
       </c>
-      <c r="D97" t="b">
-        <v>1</v>
+      <c r="D97">
+        <v>0</v>
       </c>
       <c r="E97" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F97" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I97">
         <v>0</v>
@@ -5294,7 +5298,7 @@
         <v>5</v>
       </c>
       <c r="L97" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M97">
         <v>16.5</v>
@@ -5308,19 +5312,19 @@
     </row>
     <row r="98" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B98">
         <v>329.71</v>
       </c>
-      <c r="D98" t="b">
-        <v>1</v>
+      <c r="D98">
+        <v>0</v>
       </c>
       <c r="E98" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F98" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I98">
         <v>0</v>
@@ -5332,7 +5336,7 @@
         <v>5</v>
       </c>
       <c r="L98" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M98">
         <v>36.799999999999997</v>
@@ -5346,19 +5350,19 @@
     </row>
     <row r="99" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B99">
         <v>418.13</v>
       </c>
-      <c r="D99" t="b">
-        <v>1</v>
+      <c r="D99">
+        <v>0</v>
       </c>
       <c r="E99" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F99" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I99">
         <v>0</v>
@@ -5370,7 +5374,7 @@
         <v>5</v>
       </c>
       <c r="L99" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M99">
         <v>46.4</v>
@@ -5384,19 +5388,19 @@
     </row>
     <row r="100" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B100">
         <v>552.59</v>
       </c>
-      <c r="D100" t="b">
-        <v>1</v>
+      <c r="D100">
+        <v>0</v>
       </c>
       <c r="E100" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F100" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I100">
         <v>0</v>
@@ -5408,7 +5412,7 @@
         <v>5</v>
       </c>
       <c r="L100" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M100">
         <v>55.4</v>
@@ -5422,19 +5426,19 @@
     </row>
     <row r="101" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B101">
         <v>21.07</v>
       </c>
-      <c r="D101" t="b">
-        <v>1</v>
+      <c r="D101">
+        <v>0</v>
       </c>
       <c r="E101" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F101" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I101">
         <v>0</v>
@@ -5446,7 +5450,7 @@
         <v>5</v>
       </c>
       <c r="L101" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M101">
         <v>2.2000000000000002</v>
@@ -5460,19 +5464,19 @@
     </row>
     <row r="102" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B102">
         <v>44.21</v>
       </c>
-      <c r="D102" t="b">
-        <v>1</v>
+      <c r="D102">
+        <v>0</v>
       </c>
       <c r="E102" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F102" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I102">
         <v>0</v>
@@ -5484,7 +5488,7 @@
         <v>5</v>
       </c>
       <c r="L102" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="M102">
         <v>3.35</v>
@@ -5498,19 +5502,19 @@
     </row>
     <row r="103" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B103">
         <v>61.06</v>
       </c>
-      <c r="D103" t="b">
-        <v>1</v>
+      <c r="D103">
+        <v>0</v>
       </c>
       <c r="E103" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F103" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I103">
         <v>0</v>
@@ -5522,7 +5526,7 @@
         <v>5</v>
       </c>
       <c r="L103" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M103">
         <v>5.62</v>
@@ -5536,19 +5540,19 @@
     </row>
     <row r="104" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B104">
         <v>88.41</v>
       </c>
-      <c r="D104" t="b">
-        <v>1</v>
+      <c r="D104">
+        <v>0</v>
       </c>
       <c r="E104" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F104" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I104">
         <v>0</v>
@@ -5560,7 +5564,7 @@
         <v>5</v>
       </c>
       <c r="L104" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M104">
         <v>7.9</v>
@@ -5574,19 +5578,19 @@
     </row>
     <row r="105" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B105">
         <v>142.57</v>
       </c>
-      <c r="D105" t="b">
-        <v>1</v>
+      <c r="D105">
+        <v>0</v>
       </c>
       <c r="E105" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F105" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I105">
         <v>0</v>
@@ -5598,7 +5602,7 @@
         <v>5</v>
       </c>
       <c r="L105" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M105">
         <v>12.5</v>
@@ -5612,19 +5616,19 @@
     </row>
     <row r="106" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B106">
         <v>217.35</v>
       </c>
-      <c r="D106" t="b">
-        <v>1</v>
+      <c r="D106">
+        <v>0</v>
       </c>
       <c r="E106" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F106" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I106">
         <v>0</v>
@@ -5636,7 +5640,7 @@
         <v>5</v>
       </c>
       <c r="L106" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M106">
         <v>20</v>
@@ -5650,19 +5654,19 @@
     </row>
     <row r="107" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B107">
         <v>302.08</v>
       </c>
-      <c r="D107" t="b">
-        <v>1</v>
+      <c r="D107">
+        <v>0</v>
       </c>
       <c r="E107" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F107" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I107">
         <v>0</v>
@@ -5674,7 +5678,7 @@
         <v>5</v>
       </c>
       <c r="L107" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="M107">
         <v>28.5</v>

</xml_diff>